<commit_message>
show list role in overview export
Change-Id: I575075f7fd207b30f85f97a9f763a725c2705b2c
Reviewed-on: http://gerrit.tine20.com/customers/7909
Reviewed-by: Michael Spahn <m.spahn@metaways.de>
Tested-by: Michael Spahn <m.spahn@metaways.de>
</commit_message>
<xml_diff>
--- a/tine20/Addressbook/Export/templates/addressbook_list_overview.xlsx
+++ b/tine20/Addressbook/Export/templates/addressbook_list_overview.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pzornsch/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mspahn/Workspace/tine20.com/tine20/Addressbook/Export/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24500" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="1600" windowWidth="24500" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -59,19 +59,19 @@
     <t>${twig:record.list_type}</t>
   </si>
   <si>
-    <t>${twig:record.members}</t>
-  </si>
-  <si>
     <t>${twig:translate('Name')}</t>
   </si>
   <si>
     <t>${twig:record.emails}${/ROW}</t>
+  </si>
+  <si>
+    <t>${twig:record.getListMembersWithFunctions()}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -211,11 +211,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -291,6 +291,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -312,7 +315,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Bild 2" descr="${twig:branding.logo}"/>
+        <xdr:cNvPr id="3" name="Bild 2" descr="${twig:branding.logo}">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -606,11 +615,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -658,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>8</v>
@@ -681,10 +690,10 @@
         <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>